<commit_message>
Added POR Revision Test Case
</commit_message>
<xml_diff>
--- a/GePS-HOPES_YEA/documents/MSA Files/SalesOrders_Details.xlsx
+++ b/GePS-HOPES_YEA/documents/MSA Files/SalesOrders_Details.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8550" uniqueCount="378">
   <si>
     <t>Sales Document No.</t>
   </si>
@@ -1072,6 +1072,108 @@
   </si>
   <si>
     <t>2025009770</t>
+  </si>
+  <si>
+    <t>2025002527</t>
+  </si>
+  <si>
+    <t>2025007043</t>
+  </si>
+  <si>
+    <t>2025007506</t>
+  </si>
+  <si>
+    <t>2025004241</t>
+  </si>
+  <si>
+    <t>2025004325</t>
+  </si>
+  <si>
+    <t>2025009868</t>
+  </si>
+  <si>
+    <t>202500397</t>
+  </si>
+  <si>
+    <t>2025007755</t>
+  </si>
+  <si>
+    <t>2025002681</t>
+  </si>
+  <si>
+    <t>2025004307</t>
+  </si>
+  <si>
+    <t>2025003148</t>
+  </si>
+  <si>
+    <t>2025003</t>
+  </si>
+  <si>
+    <t>2025004610</t>
+  </si>
+  <si>
+    <t>2025009590</t>
+  </si>
+  <si>
+    <t>2025007904</t>
+  </si>
+  <si>
+    <t>2025005762</t>
+  </si>
+  <si>
+    <t>2025001326</t>
+  </si>
+  <si>
+    <t>2025008525</t>
+  </si>
+  <si>
+    <t>2025006942</t>
+  </si>
+  <si>
+    <t>202500256</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>2025006186</t>
+  </si>
+  <si>
+    <t>2025009769</t>
+  </si>
+  <si>
+    <t>2025007727</t>
+  </si>
+  <si>
+    <t>2025005759</t>
+  </si>
+  <si>
+    <t>2025004784</t>
+  </si>
+  <si>
+    <t>2025001730</t>
+  </si>
+  <si>
+    <t>2025004455</t>
+  </si>
+  <si>
+    <t>2025005803</t>
+  </si>
+  <si>
+    <t>20250064</t>
+  </si>
+  <si>
+    <t>2025006655</t>
+  </si>
+  <si>
+    <t>2025006361</t>
+  </si>
+  <si>
+    <t>2025008452</t>
   </si>
 </sst>
 </file>
@@ -1145,7 +1247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1173,6 +1275,82 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -2654,7 +2832,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>343</v>
+        <v>377</v>
       </c>
       <c r="B2" t="s" s="0">
         <v>316</v>
@@ -2893,8 +3071,8 @@
       <c r="HF2" t="s" s="0">
         <v>329</v>
       </c>
-      <c r="HJ2" t="n" s="11">
-        <v>46006.0</v>
+      <c r="HJ2" t="n" s="87">
+        <v>46021.0</v>
       </c>
       <c r="HK2" t="s" s="0">
         <v>330</v>
@@ -2944,7 +3122,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>343</v>
+        <v>377</v>
       </c>
       <c r="B3" t="s" s="0">
         <v>332</v>
@@ -3183,8 +3361,8 @@
       <c r="HF3" t="s" s="0">
         <v>329</v>
       </c>
-      <c r="HJ3" t="n" s="12">
-        <v>46006.0</v>
+      <c r="HJ3" t="n" s="88">
+        <v>46021.0</v>
       </c>
       <c r="HK3" t="s" s="0">
         <v>330</v>

</xml_diff>

<commit_message>
Added SD Test Case
</commit_message>
<xml_diff>
--- a/GePS-HOPES_YEA/documents/MSA Files/SalesOrders_Details.xlsx
+++ b/GePS-HOPES_YEA/documents/MSA Files/SalesOrders_Details.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8550" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9606" uniqueCount="382">
   <si>
     <t>Sales Document No.</t>
   </si>
@@ -1174,6 +1174,18 @@
   </si>
   <si>
     <t>2025008452</t>
+  </si>
+  <si>
+    <t>2025009741</t>
+  </si>
+  <si>
+    <t>202500716</t>
+  </si>
+  <si>
+    <t>2025006653</t>
+  </si>
+  <si>
+    <t>2025002968</t>
   </si>
 </sst>
 </file>
@@ -1247,7 +1259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1275,6 +1287,17 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -1669,7 +1692,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:KF3"/>
+  <dimension ref="A1:KF4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -2832,7 +2855,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="B2" t="s" s="0">
         <v>316</v>
@@ -3071,7 +3094,7 @@
       <c r="HF2" t="s" s="0">
         <v>329</v>
       </c>
-      <c r="HJ2" t="n" s="87">
+      <c r="HJ2" t="n" s="97">
         <v>46021.0</v>
       </c>
       <c r="HK2" t="s" s="0">
@@ -3122,7 +3145,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="B3" t="s" s="0">
         <v>332</v>
@@ -3361,7 +3384,7 @@
       <c r="HF3" t="s" s="0">
         <v>329</v>
       </c>
-      <c r="HJ3" t="n" s="88">
+      <c r="HJ3" t="n" s="98">
         <v>46021.0</v>
       </c>
       <c r="HK3" t="s" s="0">
@@ -3407,6 +3430,296 @@
         <v>312</v>
       </c>
       <c r="JT3" t="s" s="0">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>381</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>364</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>291</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>292</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>293</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>317</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>315</v>
+      </c>
+      <c r="K4" t="s" s="0">
+        <v>318</v>
+      </c>
+      <c r="L4" t="s" s="0">
+        <v>294</v>
+      </c>
+      <c r="M4" t="s" s="0">
+        <v>319</v>
+      </c>
+      <c r="N4" t="s" s="0">
+        <v>295</v>
+      </c>
+      <c r="S4" t="s" s="0">
+        <v>296</v>
+      </c>
+      <c r="U4" t="s" s="0">
+        <v>334</v>
+      </c>
+      <c r="V4" t="s" s="0">
+        <v>335</v>
+      </c>
+      <c r="X4" t="s" s="0">
+        <v>297</v>
+      </c>
+      <c r="Y4" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="Z4" t="s" s="0">
+        <v>307</v>
+      </c>
+      <c r="AA4" t="s" s="0">
+        <v>314</v>
+      </c>
+      <c r="AB4" t="s" s="0">
+        <v>335</v>
+      </c>
+      <c r="AK4" t="s" s="0">
+        <v>300</v>
+      </c>
+      <c r="AM4" t="s" s="0">
+        <v>300</v>
+      </c>
+      <c r="AO4" t="s" s="0">
+        <v>320</v>
+      </c>
+      <c r="AP4" t="s" s="0">
+        <v>321</v>
+      </c>
+      <c r="AQ4" t="s" s="0">
+        <v>291</v>
+      </c>
+      <c r="BA4" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="BB4" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BG4" t="s" s="0">
+        <v>301</v>
+      </c>
+      <c r="BI4" t="s" s="0">
+        <v>291</v>
+      </c>
+      <c r="BM4" t="s" s="0">
+        <v>291</v>
+      </c>
+      <c r="BO4" t="s" s="0">
+        <v>301</v>
+      </c>
+      <c r="BW4" t="s" s="0">
+        <v>302</v>
+      </c>
+      <c r="BX4" t="s" s="0">
+        <v>303</v>
+      </c>
+      <c r="CA4" t="s" s="0">
+        <v>291</v>
+      </c>
+      <c r="CE4" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="CF4" t="s" s="0">
+        <v>322</v>
+      </c>
+      <c r="CN4" t="s" s="0">
+        <v>304</v>
+      </c>
+      <c r="CO4" t="s" s="0">
+        <v>305</v>
+      </c>
+      <c r="CP4" t="s" s="0">
+        <v>336</v>
+      </c>
+      <c r="CT4" t="s" s="0">
+        <v>290</v>
+      </c>
+      <c r="CW4" t="s" s="0">
+        <v>323</v>
+      </c>
+      <c r="DB4" t="s" s="0">
+        <v>324</v>
+      </c>
+      <c r="DD4" t="s" s="0">
+        <v>365</v>
+      </c>
+      <c r="DE4" t="s" s="0">
+        <v>326</v>
+      </c>
+      <c r="DF4" t="s" s="0">
+        <v>327</v>
+      </c>
+      <c r="DG4" t="s" s="0">
+        <v>291</v>
+      </c>
+      <c r="DI4" t="s" s="0">
+        <v>307</v>
+      </c>
+      <c r="DJ4" t="s" s="0">
+        <v>307</v>
+      </c>
+      <c r="DL4" t="s" s="0">
+        <v>291</v>
+      </c>
+      <c r="DM4" t="s" s="0">
+        <v>306</v>
+      </c>
+      <c r="DP4" t="s" s="0">
+        <v>307</v>
+      </c>
+      <c r="DS4" t="s" s="0">
+        <v>307</v>
+      </c>
+      <c r="DV4" t="s" s="0">
+        <v>307</v>
+      </c>
+      <c r="DY4" t="s" s="0">
+        <v>307</v>
+      </c>
+      <c r="EB4" t="s" s="0">
+        <v>307</v>
+      </c>
+      <c r="EJ4" t="s" s="0">
+        <v>307</v>
+      </c>
+      <c r="EM4" t="s" s="0">
+        <v>307</v>
+      </c>
+      <c r="EP4" t="s" s="0">
+        <v>307</v>
+      </c>
+      <c r="ES4" t="s" s="0">
+        <v>307</v>
+      </c>
+      <c r="EV4" t="s" s="0">
+        <v>307</v>
+      </c>
+      <c r="EW4" t="s" s="0">
+        <v>291</v>
+      </c>
+      <c r="EY4" t="s" s="0">
+        <v>307</v>
+      </c>
+      <c r="EZ4" t="s" s="0">
+        <v>291</v>
+      </c>
+      <c r="FB4" t="s" s="0">
+        <v>307</v>
+      </c>
+      <c r="FC4" t="s" s="0">
+        <v>291</v>
+      </c>
+      <c r="FE4" t="s" s="0">
+        <v>307</v>
+      </c>
+      <c r="FF4" t="s" s="0">
+        <v>291</v>
+      </c>
+      <c r="FH4" t="s" s="0">
+        <v>307</v>
+      </c>
+      <c r="FI4" t="s" s="0">
+        <v>291</v>
+      </c>
+      <c r="FK4" t="s" s="0">
+        <v>307</v>
+      </c>
+      <c r="FL4" t="s" s="0">
+        <v>307</v>
+      </c>
+      <c r="FM4" t="s" s="0">
+        <v>307</v>
+      </c>
+      <c r="FN4" t="s" s="0">
+        <v>307</v>
+      </c>
+      <c r="FO4" t="s" s="0">
+        <v>307</v>
+      </c>
+      <c r="FP4" t="s" s="0">
+        <v>307</v>
+      </c>
+      <c r="FQ4" t="s" s="0">
+        <v>307</v>
+      </c>
+      <c r="FR4" t="s" s="0">
+        <v>308</v>
+      </c>
+      <c r="FS4" t="s" s="0">
+        <v>306</v>
+      </c>
+      <c r="FT4" t="s" s="0">
+        <v>307</v>
+      </c>
+      <c r="GB4" t="s" s="7">
+        <v>328</v>
+      </c>
+      <c r="HF4" t="s" s="0">
+        <v>329</v>
+      </c>
+      <c r="HJ4" t="n" s="99">
+        <v>46021.0</v>
+      </c>
+      <c r="HK4" t="s" s="0">
+        <v>330</v>
+      </c>
+      <c r="HM4" t="s" s="0">
+        <v>309</v>
+      </c>
+      <c r="HN4" t="s" s="0">
+        <v>291</v>
+      </c>
+      <c r="IG4" t="s" s="0">
+        <v>310</v>
+      </c>
+      <c r="IH4" t="s" s="0">
+        <v>311</v>
+      </c>
+      <c r="II4" t="s" s="0">
+        <v>310</v>
+      </c>
+      <c r="IJ4" t="s" s="0">
+        <v>311</v>
+      </c>
+      <c r="IK4" t="s" s="0">
+        <v>311</v>
+      </c>
+      <c r="IL4" t="s" s="0">
+        <v>331</v>
+      </c>
+      <c r="IN4" t="s" s="0">
+        <v>311</v>
+      </c>
+      <c r="IO4" t="s" s="0">
+        <v>311</v>
+      </c>
+      <c r="IP4" t="s" s="0">
+        <v>326</v>
+      </c>
+      <c r="IQ4" t="s" s="0">
+        <v>299</v>
+      </c>
+      <c r="IR4" t="s" s="0">
+        <v>312</v>
+      </c>
+      <c r="JT4" t="s" s="0">
         <v>307</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated PS. Sales and SD Test Cases
</commit_message>
<xml_diff>
--- a/GePS-HOPES_YEA/documents/MSA Files/SalesOrders_Details.xlsx
+++ b/GePS-HOPES_YEA/documents/MSA Files/SalesOrders_Details.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9606" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14214" uniqueCount="403">
   <si>
     <t>Sales Document No.</t>
   </si>
@@ -1186,6 +1186,69 @@
   </si>
   <si>
     <t>2025002968</t>
+  </si>
+  <si>
+    <t>2025007020</t>
+  </si>
+  <si>
+    <t>2025004831</t>
+  </si>
+  <si>
+    <t>2025003511</t>
+  </si>
+  <si>
+    <t>2025002429</t>
+  </si>
+  <si>
+    <t>2025006080</t>
+  </si>
+  <si>
+    <t>2025008804</t>
+  </si>
+  <si>
+    <t>2025003891</t>
+  </si>
+  <si>
+    <t>2025005372</t>
+  </si>
+  <si>
+    <t>2025006962</t>
+  </si>
+  <si>
+    <t>2025005666</t>
+  </si>
+  <si>
+    <t>2025005626</t>
+  </si>
+  <si>
+    <t>20250046</t>
+  </si>
+  <si>
+    <t>2025002635</t>
+  </si>
+  <si>
+    <t>20250029</t>
+  </si>
+  <si>
+    <t>2025001932</t>
+  </si>
+  <si>
+    <t>202500727</t>
+  </si>
+  <si>
+    <t>2025009155</t>
+  </si>
+  <si>
+    <t>2025001872</t>
+  </si>
+  <si>
+    <t>2025003563</t>
+  </si>
+  <si>
+    <t>2025006912</t>
+  </si>
+  <si>
+    <t>2025004867</t>
   </si>
 </sst>
 </file>
@@ -1259,7 +1322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1287,6 +1350,54 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -2855,7 +2966,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>381</v>
+        <v>402</v>
       </c>
       <c r="B2" t="s" s="0">
         <v>316</v>
@@ -3094,7 +3205,7 @@
       <c r="HF2" t="s" s="0">
         <v>329</v>
       </c>
-      <c r="HJ2" t="n" s="97">
+      <c r="HJ2" t="n" s="145">
         <v>46021.0</v>
       </c>
       <c r="HK2" t="s" s="0">
@@ -3145,7 +3256,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>381</v>
+        <v>402</v>
       </c>
       <c r="B3" t="s" s="0">
         <v>332</v>
@@ -3384,7 +3495,7 @@
       <c r="HF3" t="s" s="0">
         <v>329</v>
       </c>
-      <c r="HJ3" t="n" s="98">
+      <c r="HJ3" t="n" s="146">
         <v>46021.0</v>
       </c>
       <c r="HK3" t="s" s="0">
@@ -3435,7 +3546,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>381</v>
+        <v>402</v>
       </c>
       <c r="B4" t="s" s="0">
         <v>364</v>
@@ -3674,7 +3785,7 @@
       <c r="HF4" t="s" s="0">
         <v>329</v>
       </c>
-      <c r="HJ4" t="n" s="99">
+      <c r="HJ4" t="n" s="147">
         <v>46021.0</v>
       </c>
       <c r="HK4" t="s" s="0">

</xml_diff>